<commit_message>
with errors for Story and direction corrected + var
</commit_message>
<xml_diff>
--- a/Files/Raw_Files/Design_P_ATS.xlsx
+++ b/Files/Raw_Files/Design_P_ATS.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3577F2A-8FD0-A245-9DBC-4E9211FD721C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1EAC9C-825A-844A-9A9C-71C8C4F2BB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="33600" windowHeight="19380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5 Pisos" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="65">
   <si>
     <t>X</t>
   </si>
@@ -1823,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:BQ304"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CE14" sqref="CE14"/>
+    <sheetView topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F305" sqref="F305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -37835,7 +37835,9 @@
       <c r="D189" s="72">
         <v>4</v>
       </c>
-      <c r="E189" s="72"/>
+      <c r="E189" s="72" t="s">
+        <v>0</v>
+      </c>
       <c r="F189" s="45">
         <v>1.1000000000000001</v>
       </c>
@@ -44107,7 +44109,9 @@
     </row>
     <row r="221" spans="4:69" ht="16">
       <c r="D221" s="73"/>
-      <c r="E221" s="72"/>
+      <c r="E221" s="72" t="s">
+        <v>1</v>
+      </c>
       <c r="F221" s="45" t="s">
         <v>2</v>
       </c>
@@ -49205,7 +49209,9 @@
       <c r="D247" s="72">
         <v>5</v>
       </c>
-      <c r="E247" s="72"/>
+      <c r="E247" s="72" t="s">
+        <v>0</v>
+      </c>
       <c r="F247" s="45">
         <v>1.1000000000000001</v>
       </c>
@@ -55477,7 +55483,9 @@
     </row>
     <row r="279" spans="4:69" ht="16">
       <c r="D279" s="73"/>
-      <c r="E279" s="72"/>
+      <c r="E279" s="72" t="s">
+        <v>1</v>
+      </c>
       <c r="F279" s="45" t="s">
         <v>2</v>
       </c>
@@ -60658,8 +60666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835E9031-2245-4FBC-97D9-914465FD0CB1}">
   <dimension ref="B1:AC362"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+    <sheetView tabSelected="1" topLeftCell="A327" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E279" sqref="E279:E304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -74624,7 +74632,9 @@
       <c r="D189" s="72">
         <v>4</v>
       </c>
-      <c r="E189" s="72"/>
+      <c r="E189" s="72" t="s">
+        <v>0</v>
+      </c>
       <c r="F189" s="45">
         <v>1.1000000000000001</v>
       </c>
@@ -77056,7 +77066,9 @@
     </row>
     <row r="221" spans="4:29" ht="16">
       <c r="D221" s="73"/>
-      <c r="E221" s="72"/>
+      <c r="E221" s="72" t="s">
+        <v>1</v>
+      </c>
       <c r="F221" s="45" t="s">
         <v>2</v>
       </c>
@@ -79034,7 +79046,9 @@
       <c r="D247" s="72">
         <v>5</v>
       </c>
-      <c r="E247" s="72"/>
+      <c r="E247" s="72" t="s">
+        <v>0</v>
+      </c>
       <c r="F247" s="45">
         <v>1.1000000000000001</v>
       </c>
@@ -81466,7 +81480,9 @@
     </row>
     <row r="279" spans="4:29" ht="16">
       <c r="D279" s="73"/>
-      <c r="E279" s="72"/>
+      <c r="E279" s="72" t="s">
+        <v>1</v>
+      </c>
       <c r="F279" s="45" t="s">
         <v>2</v>
       </c>

</xml_diff>